<commit_message>
Add new risk metrics, kde, and input function
</commit_message>
<xml_diff>
--- a/refined_history.xlsx
+++ b/refined_history.xlsx
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" t="n">
-        <v>13.94</v>
+        <v>13.39</v>
       </c>
       <c r="D2" t="n">
         <v>37</v>
@@ -509,19 +509,19 @@
         <v>26.32594594594595</v>
       </c>
       <c r="F2" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" t="n">
-        <v>-20.49302325581396</v>
+        <v>-20.03863636363636</v>
       </c>
       <c r="H2" t="n">
-        <v>1.16075</v>
+        <v>1.140246913580247</v>
       </c>
       <c r="I2" t="n">
-        <v>46.25</v>
+        <v>45.67901234567901</v>
       </c>
       <c r="J2" t="n">
-        <v>1.284629681883427</v>
+        <v>1.31375935309246</v>
       </c>
     </row>
     <row r="3">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>2.61</v>
+        <v>2.64</v>
       </c>
       <c r="D3" t="n">
         <v>7</v>
@@ -543,19 +543,19 @@
         <v>18.67142857142857</v>
       </c>
       <c r="F3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>-6.4375</v>
+        <v>-7.355555555555556</v>
       </c>
       <c r="H3" t="n">
-        <v>5.280000000000001</v>
+        <v>4.031250000000001</v>
       </c>
       <c r="I3" t="n">
-        <v>46.66666666666666</v>
+        <v>43.75</v>
       </c>
       <c r="J3" t="n">
-        <v>2.900416088765604</v>
+        <v>2.538411739318084</v>
       </c>
     </row>
     <row r="4">
@@ -565,31 +565,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C4" t="n">
-        <v>18.29</v>
+        <v>18.02</v>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" t="n">
-        <v>26.92595744680851</v>
+        <v>26.394375</v>
       </c>
       <c r="F4" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G4" t="n">
-        <v>-25.83103448275862</v>
+        <v>-24.79262295081967</v>
       </c>
       <c r="H4" t="n">
-        <v>-2.215999999999999</v>
+        <v>-2.25155963302752</v>
       </c>
       <c r="I4" t="n">
-        <v>44.76190476190477</v>
+        <v>44.03669724770643</v>
       </c>
       <c r="J4" t="n">
-        <v>1.042387886740685</v>
+        <v>1.064605993982874</v>
       </c>
     </row>
     <row r="5">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="n">
-        <v>7.49</v>
+        <v>7.27</v>
       </c>
       <c r="D5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="n">
-        <v>14.71454545454545</v>
+        <v>15.16086956521739</v>
       </c>
       <c r="F5" t="n">
         <v>21</v>
@@ -617,13 +617,13 @@
         <v>-10.43571428571429</v>
       </c>
       <c r="H5" t="n">
-        <v>2.431860465116277</v>
+        <v>2.944318181818179</v>
       </c>
       <c r="I5" t="n">
-        <v>51.16279069767442</v>
+        <v>52.27272727272727</v>
       </c>
       <c r="J5" t="n">
-        <v>1.410018044925642</v>
+        <v>1.452786953545814</v>
       </c>
     </row>
     <row r="6">
@@ -633,10 +633,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.52</v>
+        <v>0.66</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
@@ -645,19 +645,19 @@
         <v>17.495</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>-14</v>
+        <v>-12.45</v>
       </c>
       <c r="H6" t="n">
-        <v>6.996666666666668</v>
+        <v>2.522500000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>66.66666666666666</v>
+        <v>50</v>
       </c>
       <c r="J6" t="n">
-        <v>1.249642857142857</v>
+        <v>1.405220883534137</v>
       </c>
     </row>
     <row r="7">
@@ -670,7 +670,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>1.57</v>
+        <v>1.49</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
@@ -704,7 +704,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="n">
-        <v>3.14</v>
+        <v>2.98</v>
       </c>
       <c r="D8" t="n">
         <v>10</v>
@@ -735,10 +735,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>5.23</v>
+        <v>5.29</v>
       </c>
       <c r="D9" t="n">
         <v>16</v>
@@ -747,19 +747,19 @@
         <v>21.398125</v>
       </c>
       <c r="F9" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G9" t="n">
-        <v>-30.75714285714286</v>
+        <v>-27.540625</v>
       </c>
       <c r="H9" t="n">
-        <v>-2.941000000000003</v>
+        <v>-3.071250000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>53.33333333333334</v>
+        <v>50</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6957123780771016</v>
+        <v>0.7769658459094519</v>
       </c>
     </row>
     <row r="10">
@@ -769,31 +769,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C10" t="n">
-        <v>27.53</v>
+        <v>26.94</v>
       </c>
       <c r="D10" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E10" t="n">
-        <v>33.41885714285714</v>
+        <v>33.34958904109588</v>
       </c>
       <c r="F10" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G10" t="n">
-        <v>-32.37761363636364</v>
+        <v>-31.92866666666667</v>
       </c>
       <c r="H10" t="n">
-        <v>-3.227278481012664</v>
+        <v>-2.693619631901846</v>
       </c>
       <c r="I10" t="n">
-        <v>44.30379746835442</v>
+        <v>44.78527607361963</v>
       </c>
       <c r="J10" t="n">
-        <v>1.032159365362371</v>
+        <v>1.044503028869434</v>
       </c>
     </row>
     <row r="11">
@@ -803,31 +803,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C11" t="n">
-        <v>11.67</v>
+        <v>11.9</v>
       </c>
       <c r="D11" t="n">
+        <v>38</v>
+      </c>
+      <c r="E11" t="n">
+        <v>14.95078947368421</v>
+      </c>
+      <c r="F11" t="n">
         <v>34</v>
       </c>
-      <c r="E11" t="n">
-        <v>15.50676470588235</v>
-      </c>
-      <c r="F11" t="n">
-        <v>33</v>
-      </c>
       <c r="G11" t="n">
-        <v>-16.33818181818182</v>
+        <v>-15.93735294117647</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.1780597014925345</v>
+        <v>0.3647222222222224</v>
       </c>
       <c r="I11" t="n">
-        <v>50.74626865671642</v>
+        <v>52.77777777777778</v>
       </c>
       <c r="J11" t="n">
-        <v>0.949112017386523</v>
+        <v>0.9380974073214298</v>
       </c>
     </row>
     <row r="12">
@@ -837,31 +837,31 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="D12" t="n">
         <v>4</v>
       </c>
-      <c r="C12" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D12" t="n">
-        <v>3</v>
-      </c>
       <c r="E12" t="n">
-        <v>1.326666666666667</v>
+        <v>4.67</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>-14.3</v>
+        <v>-14.45</v>
       </c>
       <c r="H12" t="n">
-        <v>-2.58</v>
+        <v>-1.703333333333333</v>
       </c>
       <c r="I12" t="n">
-        <v>75</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="J12" t="n">
-        <v>0.09277389277389277</v>
+        <v>0.3231833910034602</v>
       </c>
     </row>
     <row r="13">
@@ -871,16 +871,16 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D13" t="n">
         <v>2</v>
       </c>
-      <c r="C13" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
       <c r="E13" t="n">
-        <v>2.7</v>
+        <v>2.55</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -889,13 +889,13 @@
         <v>-2.75</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.02499999999999991</v>
+        <v>0.7833333333333331</v>
       </c>
       <c r="I13" t="n">
-        <v>50</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="J13" t="n">
-        <v>0.9818181818181819</v>
+        <v>0.9272727272727272</v>
       </c>
     </row>
     <row r="14">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>0.87</v>
+        <v>0.99</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -917,13 +917,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14" t="n">
-        <v>-11.75</v>
+        <v>-10.40833333333333</v>
       </c>
       <c r="H14" t="n">
-        <v>-11.75</v>
+        <v>-10.40833333333333</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -942,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -973,10 +973,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>0.17</v>
+        <v>0.66</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -985,16 +985,19 @@
         <v>7.22</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>-1.37</v>
       </c>
       <c r="H16" t="n">
-        <v>7.22</v>
+        <v>0.7775000000000001</v>
       </c>
       <c r="I16" t="n">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.27007299270073</v>
       </c>
     </row>
     <row r="17">
@@ -1007,7 +1010,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>2.26</v>
+        <v>2.15</v>
       </c>
       <c r="D17" t="n">
         <v>5</v>
@@ -1072,7 +1075,7 @@
         <v>11</v>
       </c>
       <c r="C19" t="n">
-        <v>1.92</v>
+        <v>1.82</v>
       </c>
       <c r="D19" t="n">
         <v>4</v>
@@ -1103,10 +1106,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1115,13 +1118,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" t="n">
-        <v>-13.75</v>
+        <v>-9.243333333333334</v>
       </c>
       <c r="H20" t="n">
-        <v>-13.75</v>
+        <v>-9.243333333333334</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1171,10 +1174,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>0.17</v>
+        <v>0.66</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -1183,16 +1186,19 @@
         <v>20</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>-1.92</v>
       </c>
       <c r="H22" t="n">
-        <v>20</v>
+        <v>3.56</v>
       </c>
       <c r="I22" t="n">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="J22" t="n">
+        <v>10.41666666666667</v>
       </c>
     </row>
     <row r="23">
@@ -1237,7 +1243,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5226480836236934</v>
+        <v>0.4958677685950413</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -1391,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3484320557491289</v>
+        <v>0.3305785123966942</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
@@ -1441,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.5226480836236934</v>
+        <v>0.4958677685950413</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
@@ -1497,7 +1503,7 @@
         <v>64</v>
       </c>
       <c r="C5" t="n">
-        <v>11.14982578397213</v>
+        <v>10.57851239669422</v>
       </c>
       <c r="D5" t="n">
         <v>33</v>
@@ -1553,7 +1559,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.045296167247387</v>
+        <v>0.9917355371900827</v>
       </c>
       <c r="D6" t="n">
         <v>2</v>
@@ -1565,7 +1571,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="n">
-        <v>-37.67999999999999</v>
+        <v>-37.68</v>
       </c>
       <c r="H6" t="n">
         <v>33.33333333333333</v>
@@ -1574,16 +1580,16 @@
         <v>66.66666666666666</v>
       </c>
       <c r="J6" t="n">
-        <v>-16.24499999999999</v>
+        <v>-16.245</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7066082802547772</v>
+        <v>0.7066082802547771</v>
       </c>
       <c r="L6" t="n">
         <v>3.3</v>
       </c>
       <c r="M6" t="n">
-        <v>0.55</v>
+        <v>0.5499999999999999</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1609,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5226480836236934</v>
+        <v>0.4958677685950413</v>
       </c>
       <c r="D7" t="n">
         <v>2</v>
@@ -1665,7 +1671,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3484320557491289</v>
+        <v>0.3305785123966942</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -1721,7 +1727,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="n">
-        <v>5.052264808362369</v>
+        <v>4.793388429752066</v>
       </c>
       <c r="D9" t="n">
         <v>17</v>
@@ -1742,7 +1748,7 @@
         <v>41.37931034482759</v>
       </c>
       <c r="J9" t="n">
-        <v>4.407586206896551</v>
+        <v>4.407586206896553</v>
       </c>
       <c r="K9" t="n">
         <v>1.482152527190004</v>
@@ -1751,7 +1757,7 @@
         <v>11.3</v>
       </c>
       <c r="M9" t="n">
-        <v>0.3896551724137931</v>
+        <v>0.389655172413793</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1777,7 +1783,7 @@
         <v>86</v>
       </c>
       <c r="C10" t="n">
-        <v>14.98257839721254</v>
+        <v>14.21487603305785</v>
       </c>
       <c r="D10" t="n">
         <v>42</v>
@@ -1833,7 +1839,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>1.393728222996516</v>
+        <v>1.322314049586777</v>
       </c>
       <c r="D11" t="n">
         <v>5</v>
@@ -1854,7 +1860,7 @@
         <v>37.5</v>
       </c>
       <c r="J11" t="n">
-        <v>8.166250000000002</v>
+        <v>8.166249999999998</v>
       </c>
       <c r="K11" t="n">
         <v>1.350344563552833</v>
@@ -1889,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1742160278745645</v>
+        <v>0.1652892561983471</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -1939,7 +1945,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>1.219512195121951</v>
+        <v>1.15702479338843</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
@@ -1951,7 +1957,7 @@
         <v>5</v>
       </c>
       <c r="G13" t="n">
-        <v>-27.88200000000001</v>
+        <v>-27.882</v>
       </c>
       <c r="H13" t="n">
         <v>28.57142857142857</v>
@@ -1963,7 +1969,7 @@
         <v>-16.55857142857143</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4214188365253568</v>
+        <v>0.4214188365253569</v>
       </c>
       <c r="L13" t="n">
         <v>9.199999999999999</v>
@@ -1995,7 +2001,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>6.271777003484321</v>
+        <v>5.950413223140496</v>
       </c>
       <c r="D14" t="n">
         <v>10</v>
@@ -2051,7 +2057,7 @@
         <v>67</v>
       </c>
       <c r="C15" t="n">
-        <v>11.67247386759582</v>
+        <v>11.07438016528926</v>
       </c>
       <c r="D15" t="n">
         <v>29</v>
@@ -2072,10 +2078,10 @@
         <v>56.71641791044776</v>
       </c>
       <c r="J15" t="n">
-        <v>7.910895522388059</v>
+        <v>7.910895522388056</v>
       </c>
       <c r="K15" t="n">
-        <v>2.772373433525743</v>
+        <v>2.772373433525742</v>
       </c>
       <c r="L15" t="n">
         <v>61.8</v>
@@ -2107,7 +2113,7 @@
         <v>93</v>
       </c>
       <c r="C16" t="n">
-        <v>16.2020905923345</v>
+        <v>15.37190082644628</v>
       </c>
       <c r="D16" t="n">
         <v>42</v>
@@ -2119,7 +2125,7 @@
         <v>51</v>
       </c>
       <c r="G16" t="n">
-        <v>-3.778823529411765</v>
+        <v>-3.778823529411764</v>
       </c>
       <c r="H16" t="n">
         <v>45.16129032258064</v>
@@ -2128,16 +2134,16 @@
         <v>54.83870967741935</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.2387096774193547</v>
+        <v>-0.2387096774193542</v>
       </c>
       <c r="K16" t="n">
         <v>1.074408468244085</v>
       </c>
       <c r="L16" t="n">
-        <v>56.10000000000001</v>
+        <v>56.09999999999997</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6032258064516129</v>
+        <v>0.6032258064516126</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -2163,7 +2169,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="n">
-        <v>3.13588850174216</v>
+        <v>2.975206611570248</v>
       </c>
       <c r="D17" t="n">
         <v>6</v>
@@ -2219,13 +2225,13 @@
         <v>15</v>
       </c>
       <c r="C18" t="n">
-        <v>2.613240418118467</v>
+        <v>2.479338842975207</v>
       </c>
       <c r="D18" t="n">
         <v>7</v>
       </c>
       <c r="E18" t="n">
-        <v>105.5628571428571</v>
+        <v>105.5628571428572</v>
       </c>
       <c r="F18" t="n">
         <v>8</v>
@@ -2240,7 +2246,7 @@
         <v>53.33333333333334</v>
       </c>
       <c r="J18" t="n">
-        <v>9.323333333333331</v>
+        <v>9.323333333333338</v>
       </c>
       <c r="K18" t="n">
         <v>1.409642720030141</v>
@@ -2275,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C19" t="n">
-        <v>2.787456445993032</v>
+        <v>2.644628099173554</v>
       </c>
       <c r="D19" t="n">
         <v>10</v>
@@ -2331,13 +2337,13 @@
         <v>115</v>
       </c>
       <c r="C20" t="n">
-        <v>20.03484320557491</v>
+        <v>19.00826446280992</v>
       </c>
       <c r="D20" t="n">
         <v>51</v>
       </c>
       <c r="E20" t="n">
-        <v>15.63705882352942</v>
+        <v>15.63705882352941</v>
       </c>
       <c r="F20" t="n">
         <v>64</v>
@@ -2352,10 +2358,10 @@
         <v>55.65217391304348</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.7063478260869553</v>
+        <v>-0.7063478260869571</v>
       </c>
       <c r="K20" t="n">
-        <v>1.138897219485027</v>
+        <v>1.138897219485026</v>
       </c>
       <c r="L20" t="n">
         <v>93.2</v>
@@ -2374,6 +2380,62 @@
         </is>
       </c>
       <c r="P20" t="inlineStr">
+        <is>
+          <t>NKY</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45637</v>
+      </c>
+      <c r="B21" t="n">
+        <v>31</v>
+      </c>
+      <c r="C21" t="n">
+        <v>5.12396694214876</v>
+      </c>
+      <c r="D21" t="n">
+        <v>11</v>
+      </c>
+      <c r="E21" t="n">
+        <v>16.32636363636364</v>
+      </c>
+      <c r="F21" t="n">
+        <v>20</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-5.288</v>
+      </c>
+      <c r="H21" t="n">
+        <v>35.48387096774194</v>
+      </c>
+      <c r="I21" t="n">
+        <v>64.51612903225806</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2.381612903225807</v>
+      </c>
+      <c r="K21" t="n">
+        <v>3.087436391142897</v>
+      </c>
+      <c r="L21" t="n">
+        <v>21</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.6774193548387096</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>SX5E</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>NKY</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
         <is>
           <t>NKY</t>
         </is>

</xml_diff>